<commit_message>
- Recherche produit OK. - Thème UI Dark - Nombreuses amélmiorations UI.
</commit_message>
<xml_diff>
--- a/EIEx/EIEx/Données/BET EIE Renseigné V1 - CI_DCE_G_DPGF-13_ELECTRICITE CF&Cf.xlsx
+++ b/EIEx/EIEx/Données/BET EIE Renseigné V1 - CI_DCE_G_DPGF-13_ELECTRICITE CF&Cf.xlsx
@@ -20,6 +20,10 @@
     <sheet name="BATIMENT SOHO-ELEC 2" sheetId="31" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'BATIMENT G1,G2&amp;PKINGS-ELEC 1'!$A$14:$F$365</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'BATIMENT G1,G2&amp;PKINGS-ELEC 2'!$A$14:$F$394</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'BATIMENT SOHO-ELEC 1'!$A$14:$F$286</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'BATIMENT SOHO-ELEC 2'!$A$14:$F$186</definedName>
     <definedName name="aa" localSheetId="4">#REF!</definedName>
     <definedName name="aa" localSheetId="5">#REF!</definedName>
     <definedName name="aa">#REF!</definedName>
@@ -44,6 +48,10 @@
     <definedName name="CONNEXES">#REF!</definedName>
     <definedName name="cons_POLE_1">#REF!</definedName>
     <definedName name="COURANTS_FAIBLES">#REF!</definedName>
+    <definedName name="Data1">'BATIMENT G1,G2&amp;PKINGS-ELEC 1'!$A$14:$F$365</definedName>
+    <definedName name="Data2">'BATIMENT G1,G2&amp;PKINGS-ELEC 2'!$A$14:$F$425</definedName>
+    <definedName name="Data3">'BATIMENT SOHO-ELEC 1'!$A$14:$F$286</definedName>
+    <definedName name="Data4">'BATIMENT SOHO-ELEC 2'!$A$14:$F$186</definedName>
     <definedName name="ENDO">#REF!</definedName>
     <definedName name="FEDERATION_DES_LABORATOIRES">#REF!</definedName>
     <definedName name="HDJ">#REF!</definedName>
@@ -3824,8 +3832,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P366"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -3843,13 +3853,13 @@
     <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13">
+    <row r="1" spans="1:10" ht="13" hidden="1">
       <c r="G1" s="154"/>
       <c r="H1" s="155"/>
       <c r="I1" s="156"/>
       <c r="J1" s="157"/>
     </row>
-    <row r="2" spans="1:10" ht="13">
+    <row r="2" spans="1:10" ht="13" hidden="1">
       <c r="G2" s="158" t="s">
         <v>470</v>
       </c>
@@ -3863,7 +3873,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13">
+    <row r="3" spans="1:10" ht="13" hidden="1">
       <c r="G3" s="158" t="s">
         <v>472</v>
       </c>
@@ -3877,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14">
+    <row r="4" spans="1:10" ht="14" hidden="1">
       <c r="G4" s="158"/>
       <c r="H4" s="163" t="s">
         <v>474</v>
@@ -3888,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14">
+    <row r="5" spans="1:10" ht="14" hidden="1">
       <c r="G5" s="163"/>
       <c r="H5" s="163" t="s">
         <v>475</v>
@@ -3899,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14">
+    <row r="6" spans="1:10" ht="14" hidden="1">
       <c r="G6" s="163"/>
       <c r="H6" s="163" t="s">
         <v>476</v>
@@ -3910,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14">
+    <row r="7" spans="1:10" ht="14" hidden="1">
       <c r="G7" s="163"/>
       <c r="H7" s="163" t="s">
         <v>477</v>
@@ -3921,19 +3931,19 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14">
+    <row r="8" spans="1:10" ht="14" hidden="1">
       <c r="G8" s="163"/>
       <c r="H8" s="163"/>
       <c r="I8" s="163"/>
       <c r="J8" s="163"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="G9" s="154"/>
       <c r="H9" s="154"/>
       <c r="I9" s="154"/>
       <c r="J9" s="154"/>
     </row>
-    <row r="10" spans="1:10" ht="13" thickBot="1">
+    <row r="10" spans="1:10" ht="13" hidden="1" thickBot="1">
       <c r="G10" s="154"/>
       <c r="H10" s="154"/>
       <c r="I10" s="154"/>
@@ -13212,6 +13222,7 @@
       <c r="F366" s="51"/>
     </row>
   </sheetData>
+  <autoFilter ref="A14:F365"/>
   <mergeCells count="9">
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="B14:B15"/>
@@ -13252,8 +13263,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W394"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageBreakPreview" topLeftCell="A368" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D183" sqref="D183:J387"/>
+    <sheetView showZeros="0" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -13273,13 +13286,13 @@
     <col min="13" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13">
+    <row r="1" spans="1:10" ht="13" hidden="1">
       <c r="G1" s="154"/>
       <c r="H1" s="155"/>
       <c r="I1" s="156"/>
       <c r="J1" s="157"/>
     </row>
-    <row r="2" spans="1:10" ht="13">
+    <row r="2" spans="1:10" ht="13" hidden="1">
       <c r="G2" s="158" t="s">
         <v>470</v>
       </c>
@@ -13293,7 +13306,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13">
+    <row r="3" spans="1:10" ht="13" hidden="1">
       <c r="G3" s="158" t="s">
         <v>472</v>
       </c>
@@ -13307,7 +13320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14">
+    <row r="4" spans="1:10" ht="14" hidden="1">
       <c r="G4" s="158"/>
       <c r="H4" s="163" t="s">
         <v>474</v>
@@ -13318,7 +13331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14">
+    <row r="5" spans="1:10" ht="14" hidden="1">
       <c r="G5" s="163"/>
       <c r="H5" s="163" t="s">
         <v>475</v>
@@ -13329,7 +13342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14">
+    <row r="6" spans="1:10" ht="14" hidden="1">
       <c r="G6" s="163"/>
       <c r="H6" s="163" t="s">
         <v>476</v>
@@ -13340,7 +13353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14">
+    <row r="7" spans="1:10" ht="14" hidden="1">
       <c r="G7" s="163"/>
       <c r="H7" s="163" t="s">
         <v>477</v>
@@ -13351,19 +13364,19 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14">
+    <row r="8" spans="1:10" ht="14" hidden="1">
       <c r="G8" s="163"/>
       <c r="H8" s="163"/>
       <c r="I8" s="163"/>
       <c r="J8" s="163"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="G9" s="154"/>
       <c r="H9" s="154"/>
       <c r="I9" s="154"/>
       <c r="J9" s="154"/>
     </row>
-    <row r="10" spans="1:10" ht="13" thickBot="1">
+    <row r="10" spans="1:10" ht="13" hidden="1" thickBot="1">
       <c r="G10" s="154"/>
       <c r="H10" s="154"/>
       <c r="I10" s="154"/>
@@ -23721,6 +23734,7 @@
       <c r="F394" s="122"/>
     </row>
   </sheetData>
+  <autoFilter ref="A14:F394"/>
   <mergeCells count="9">
     <mergeCell ref="A392:E392"/>
     <mergeCell ref="A394:E394"/>
@@ -23758,8 +23772,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P287"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="L265" sqref="L265"/>
+    <sheetView showZeros="0" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -23777,13 +23793,13 @@
     <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13">
+    <row r="1" spans="1:10" ht="13" hidden="1">
       <c r="G1" s="154"/>
       <c r="H1" s="155"/>
       <c r="I1" s="156"/>
       <c r="J1" s="157"/>
     </row>
-    <row r="2" spans="1:10" ht="13">
+    <row r="2" spans="1:10" ht="13" hidden="1">
       <c r="G2" s="158" t="s">
         <v>470</v>
       </c>
@@ -23797,7 +23813,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13">
+    <row r="3" spans="1:10" ht="13" hidden="1">
       <c r="G3" s="158" t="s">
         <v>472</v>
       </c>
@@ -23811,7 +23827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14">
+    <row r="4" spans="1:10" ht="14" hidden="1">
       <c r="G4" s="158"/>
       <c r="H4" s="163" t="s">
         <v>474</v>
@@ -23822,7 +23838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14">
+    <row r="5" spans="1:10" ht="14" hidden="1">
       <c r="G5" s="163"/>
       <c r="H5" s="163" t="s">
         <v>475</v>
@@ -23833,7 +23849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14">
+    <row r="6" spans="1:10" ht="14" hidden="1">
       <c r="G6" s="163"/>
       <c r="H6" s="163" t="s">
         <v>476</v>
@@ -23844,7 +23860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14">
+    <row r="7" spans="1:10" ht="14" hidden="1">
       <c r="G7" s="163"/>
       <c r="H7" s="163" t="s">
         <v>477</v>
@@ -23855,19 +23871,19 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14">
+    <row r="8" spans="1:10" ht="14" hidden="1">
       <c r="G8" s="163"/>
       <c r="H8" s="163"/>
       <c r="I8" s="163"/>
       <c r="J8" s="163"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="G9" s="154"/>
       <c r="H9" s="154"/>
       <c r="I9" s="154"/>
       <c r="J9" s="154"/>
     </row>
-    <row r="10" spans="1:10" ht="13" thickBot="1">
+    <row r="10" spans="1:10" ht="13" hidden="1" thickBot="1">
       <c r="G10" s="154"/>
       <c r="H10" s="154"/>
       <c r="I10" s="154"/>
@@ -31001,6 +31017,7 @@
       <c r="F287" s="51"/>
     </row>
   </sheetData>
+  <autoFilter ref="A14:F286"/>
   <mergeCells count="9">
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="A282:E282"/>
@@ -31040,8 +31057,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W192"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView showZeros="0" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -31061,13 +31080,13 @@
     <col min="13" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13">
+    <row r="1" spans="1:10" ht="13" hidden="1">
       <c r="G1" s="154"/>
       <c r="H1" s="155"/>
       <c r="I1" s="156"/>
       <c r="J1" s="157"/>
     </row>
-    <row r="2" spans="1:10" ht="13">
+    <row r="2" spans="1:10" ht="13" hidden="1">
       <c r="G2" s="158" t="s">
         <v>470</v>
       </c>
@@ -31081,7 +31100,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13">
+    <row r="3" spans="1:10" ht="13" hidden="1">
       <c r="G3" s="158" t="s">
         <v>472</v>
       </c>
@@ -31095,7 +31114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14">
+    <row r="4" spans="1:10" ht="14" hidden="1">
       <c r="G4" s="158"/>
       <c r="H4" s="163" t="s">
         <v>474</v>
@@ -31106,7 +31125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14">
+    <row r="5" spans="1:10" ht="14" hidden="1">
       <c r="G5" s="163"/>
       <c r="H5" s="163" t="s">
         <v>475</v>
@@ -31117,7 +31136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14">
+    <row r="6" spans="1:10" ht="14" hidden="1">
       <c r="G6" s="163"/>
       <c r="H6" s="163" t="s">
         <v>476</v>
@@ -31128,7 +31147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14">
+    <row r="7" spans="1:10" ht="14" hidden="1">
       <c r="G7" s="163"/>
       <c r="H7" s="163" t="s">
         <v>477</v>
@@ -31139,19 +31158,19 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14">
+    <row r="8" spans="1:10" ht="14" hidden="1">
       <c r="G8" s="163"/>
       <c r="H8" s="163"/>
       <c r="I8" s="163"/>
       <c r="J8" s="163"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="G9" s="154"/>
       <c r="H9" s="154"/>
       <c r="I9" s="154"/>
       <c r="J9" s="154"/>
     </row>
-    <row r="10" spans="1:10" ht="13" thickBot="1">
+    <row r="10" spans="1:10" ht="13" hidden="1" thickBot="1">
       <c r="G10" s="154"/>
       <c r="H10" s="154"/>
       <c r="I10" s="154"/>
@@ -35857,6 +35876,7 @@
       <c r="F192" s="122"/>
     </row>
   </sheetData>
+  <autoFilter ref="A14:F186"/>
   <mergeCells count="8">
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="A192:E192"/>

</xml_diff>